<commit_message>
finished with a slight error
</commit_message>
<xml_diff>
--- a/src/tk_dn1_63190277/Belezke.xlsx
+++ b/src/tk_dn1_63190277/Belezke.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\GitHub\TK\src\tk_dn1_63190277\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADBC44B-1D0B-4F13-A42D-14C8C7A8C8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46E5913-B33B-4BAC-B17C-D35309A76831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2EBF3EAA-E479-4901-BD4B-FC95096E004B}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -383,7 +383,7 @@
   <rv s="0">
     <v>0</v>
     <v>8</v>
-    <v>1</v>
+    <v>2</v>
     <v>5</v>
   </rv>
   <rv s="1">
@@ -462,8 +462,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E25FD3EA-4233-4225-AC21-0FAFF61DE916}" name="Tabela2" displayName="Tabela2" ref="A1:K3" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:K3" xr:uid="{E25FD3EA-4233-4225-AC21-0FAFF61DE916}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E25FD3EA-4233-4225-AC21-0FAFF61DE916}" name="Tabela2" displayName="Tabela2" ref="A1:K4" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:K4" xr:uid="{E25FD3EA-4233-4225-AC21-0FAFF61DE916}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{6F33A7BB-6D56-4319-9C17-36B417C75F66}" name="ID"/>
     <tableColumn id="2" xr3:uid="{51D35727-ACE4-41C5-A92E-613241A72508}" name="Opravilo"/>
@@ -484,8 +484,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{289923E5-C8DB-4D41-A8F2-3F18C56B7C5A}" name="Tabela5" displayName="Tabela5" ref="A1:K3" totalsRowShown="0">
-  <autoFilter ref="A1:K3" xr:uid="{289923E5-C8DB-4D41-A8F2-3F18C56B7C5A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{289923E5-C8DB-4D41-A8F2-3F18C56B7C5A}" name="Tabela5" displayName="Tabela5" ref="A1:K4" totalsRowShown="0">
+  <autoFilter ref="A1:K4" xr:uid="{289923E5-C8DB-4D41-A8F2-3F18C56B7C5A}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{24BA900E-2054-4A20-AE15-4C15867E4D74}" name="ID"/>
     <tableColumn id="2" xr3:uid="{446A6F87-BFB7-46FB-B479-8817977CC696}" name="Opravilo"/>
@@ -805,7 +805,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,9 +1301,27 @@
       <c r="D14">
         <v>7</v>
       </c>
+      <c r="E14">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>7</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
       <c r="K14">
         <f>SUM(Tabela1[[#This Row],[Planiranje]:[Analiza]])</f>
-        <v>13</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1320,11 +1338,11 @@
       </c>
       <c r="E15">
         <f>SUBTOTAL(109,Tabela1[Testi])</f>
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F15">
         <f>SUBTOTAL(109,Tabela1[Programiranje])</f>
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="G15">
         <f>SUBTOTAL(109,Tabela1[Pregled])</f>
@@ -1336,7 +1354,7 @@
       </c>
       <c r="I15">
         <f>SUBTOTAL(109,Tabela1[Testiranje])</f>
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J15">
         <f>SUBTOTAL(109,Tabela1[Analiza])</f>
@@ -1344,7 +1362,7 @@
       </c>
       <c r="K15">
         <f>SUBTOTAL(109,Tabela1[Skupaj])</f>
-        <v>229</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -1360,7 +1378,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1870,29 +1888,35 @@
       <c r="B14" t="s">
         <v>33</v>
       </c>
+      <c r="C14">
+        <v>63</v>
+      </c>
+      <c r="D14">
+        <v>29</v>
+      </c>
       <c r="E14" s="6">
         <f>SUM(Tabela3[[#This Row],[LOC_Testi]:[LOC_Program]])</f>
-        <v>0</v>
-      </c>
-      <c r="F14" t="e">
+        <v>92</v>
+      </c>
+      <c r="F14">
         <f>SUMIF(Tabela1[ID],Tabela3[[#This Row],[ID]],Tabela1[Skupaj])/Tabela3[[#This Row],[LOC]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G14" t="e">
+        <v>0.56521739130434778</v>
+      </c>
+      <c r="G14">
         <f>60/Tabela3[[#This Row],[Min/LOC]]</f>
-        <v>#DIV/0!</v>
+        <v>106.15384615384616</v>
       </c>
       <c r="H14" t="e" cm="1" vm="1">
         <f t="array" aca="1" ref="H14" ca="1">1000*(Tabela2[Skupaj]/Tabela3[[#This Row],[LOC]])</f>
         <v>#VALUE!</v>
       </c>
-      <c r="I14" t="e">
+      <c r="I14">
         <f>100*SUM(SUMIF(Tabela5[ID],Tabela3[[#This Row],[ID]],Tabela5[Planiranje]),SUMIF(Tabela5[ID],Tabela3[[#This Row],[ID]],Tabela5[Načrtovanje]),SUMIF(Tabela5[ID],Tabela3[[#This Row],[ID]],Tabela5[Testi]),SUMIF(Tabela5[ID],Tabela3[[#This Row],[ID]],Tabela5[Programiranje]),SUMIF(Tabela5[ID],Tabela3[[#This Row],[ID]],Tabela5[Pregled]),)/SUM(SUMIF(Tabela2[ID],Tabela3[[#This Row],[ID]],Tabela2[Planiranje]),SUMIF(Tabela2[ID],Tabela3[[#This Row],[ID]],Tabela2[Načrtovanje]),SUMIF(Tabela2[ID],Tabela3[[#This Row],[ID]],Tabela2[Testi]),SUMIF(Tabela2[ID],Tabela3[[#This Row],[ID]],Tabela2[Programiranje]), SUMIF(Tabela2[ID],Tabela3[[#This Row],[ID]],Tabela2[Pregled]))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J14" t="e">
+        <v>0</v>
+      </c>
+      <c r="J14">
         <f>SUMIF(Tabela1[ID],Tabela3[[#This Row],[ID]],Tabela1[Pregled])/(SUMIF(Tabela1[ID],Tabela3[[#This Row],[ID]],Tabela1[Prevajanje])+SUMIF(Tabela1[ID],Tabela3[[#This Row],[ID]],Tabela1[Testiranje]))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1901,23 +1925,23 @@
       </c>
       <c r="C15">
         <f>SUBTOTAL(109,Tabela3[LOC_Testi])</f>
-        <v>279</v>
+        <v>342</v>
       </c>
       <c r="D15">
         <f>SUBTOTAL(109,Tabela3[LOC_Program])</f>
-        <v>237</v>
+        <v>266</v>
       </c>
       <c r="E15">
         <f>SUBTOTAL(109,Tabela3[LOC])</f>
-        <v>516</v>
-      </c>
-      <c r="F15" t="e">
+        <v>608</v>
+      </c>
+      <c r="F15">
         <f>SUBTOTAL(101,Tabela3[Min/LOC])</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G15" t="e">
+        <v>0.44387385902000875</v>
+      </c>
+      <c r="G15">
         <f>SUBTOTAL(101,Tabela3[LOC/Uro])</f>
-        <v>#DIV/0!</v>
+        <v>393.68347738619366</v>
       </c>
       <c r="H15" t="e" vm="2">
         <f ca="1">SUBTOTAL(101,Tabela3[napake/KLOC])</f>
@@ -1942,9 +1966,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1340E9-BA89-4E22-A618-FED12E15F5E2}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="A4:B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2065,6 +2091,42 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f>SUM(Tabela2[[#This Row],[Planiranje]:[Analiza]])</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2075,10 +2137,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A374FAC9-BDF0-4E90-9F43-90EA2ED21369}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2156,6 +2218,9 @@
       <c r="I2">
         <v>3</v>
       </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
       <c r="K2">
         <f>SUM(Tabela5[[#This Row],[Planiranje]:[Analiza]])</f>
         <v>4</v>
@@ -2168,15 +2233,69 @@
       <c r="B3" t="s">
         <v>32</v>
       </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
       <c r="G3">
         <v>3</v>
       </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
       </c>
       <c r="K3">
         <f>SUM(Tabela5[[#This Row],[Planiranje]:[Analiza]])</f>
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f>SUM(Tabela5[[#This Row],[Planiranje]:[Analiza]])</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>